<commit_message>
Fix error in reading GAMS parameters
Two lines had errors when trying to read in GAMS parameters. This hard codes the `damadj` term (not used in GAMS) to 1 and adds the `eqmat` term to the parameter excel file.
</commit_message>
<xml_diff>
--- a/data/DICE2013_IAMF_Parameters.xlsx
+++ b/data/DICE2013_IAMF_Parameters.xlsx
@@ -1,16 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frank Errickson\Desktop\Git_Folders\FIX_DICE_GAMS\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E88D5A-52AC-490F-AD21-370E77F86829}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24700" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DICE2013_Base" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Year</t>
   </si>
@@ -166,12 +178,15 @@
   </si>
   <si>
     <t>scale2</t>
+  </si>
+  <si>
+    <t>eqmat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="#,##0.00000_);\(#,##0.00000\)"/>
@@ -286,6 +301,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -610,20 +633,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BP57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BP58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.5" customWidth="1"/>
     <col min="57" max="57" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61">
+    <row r="1" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -808,7 +831,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:61">
+    <row r="2" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -993,12 +1016,12 @@
         <v>2305</v>
       </c>
     </row>
-    <row r="4" spans="1:61">
+    <row r="4" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:61">
+    <row r="5" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1183,7 +1206,7 @@
         <v>36.845992238896798</v>
       </c>
     </row>
-    <row r="6" spans="1:61">
+    <row r="6" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1368,7 +1391,7 @@
         <v>10499.0730388837</v>
       </c>
     </row>
-    <row r="7" spans="1:61">
+    <row r="7" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1376,7 +1399,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="8" spans="1:61">
+    <row r="8" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1384,7 +1407,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:61">
+    <row r="9" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1392,12 +1415,12 @@
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="1:61">
+    <row r="11" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:61">
+    <row r="12" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1582,7 +1605,7 @@
         <v>4.2412052770377899E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:61">
+    <row r="13" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1767,7 +1790,7 @@
         <v>6.3215441060718098E-6</v>
       </c>
     </row>
-    <row r="14" spans="1:61">
+    <row r="14" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -1775,12 +1798,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:61">
+    <row r="16" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:61">
+    <row r="17" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1788,7 +1811,7 @@
         <v>830.4</v>
       </c>
     </row>
-    <row r="18" spans="1:61">
+    <row r="18" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1796,7 +1819,7 @@
         <v>1527</v>
       </c>
     </row>
-    <row r="19" spans="1:61">
+    <row r="19" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1804,7 +1827,7 @@
         <v>10010</v>
       </c>
     </row>
-    <row r="20" spans="1:61">
+    <row r="20" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -1812,7 +1835,7 @@
         <v>8.7999999999999995E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:61">
+    <row r="21" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -1820,7 +1843,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:61">
+    <row r="22" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1829,7 +1852,7 @@
         <v>0.91200000000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:61">
+    <row r="23" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -1838,7 +1861,7 @@
         <v>3.8328888888888885E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:61">
+    <row r="24" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -1847,7 +1870,7 @@
         <v>0.9591711111111112</v>
       </c>
     </row>
-    <row r="25" spans="1:61">
+    <row r="25" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -1856,7 +1879,7 @@
         <v>3.3750000000000002E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:61">
+    <row r="26" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -1865,12 +1888,12 @@
         <v>0.99966250000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:61">
+    <row r="28" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:61">
+    <row r="29" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -2055,7 +2078,7 @@
         <v>1.7249999999999901</v>
       </c>
     </row>
-    <row r="30" spans="1:61">
+    <row r="30" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -2063,1245 +2086,1253 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="32" spans="1:61">
-      <c r="A32" t="s">
+    <row r="31" spans="1:61" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="33" spans="1:61" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:61">
-      <c r="A33" t="s">
+    <row r="34" spans="1:61" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>26</v>
       </c>
-      <c r="B33">
+      <c r="B34">
         <v>2.9</v>
       </c>
     </row>
-    <row r="34" spans="1:61">
-      <c r="A34" t="s">
+    <row r="35" spans="1:61" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>27</v>
       </c>
-      <c r="B34">
+      <c r="B35">
         <v>0.8</v>
       </c>
     </row>
-    <row r="35" spans="1:61">
-      <c r="A35" t="s">
+    <row r="36" spans="1:61" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>28</v>
       </c>
-      <c r="B35">
+      <c r="B36">
         <v>6.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:61">
-      <c r="A36" t="s">
+    <row r="37" spans="1:61" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>29</v>
       </c>
-      <c r="B36">
-        <f>0.098+0.01243*(B33-2.9)</f>
+      <c r="B37">
+        <f>0.098+0.01243*(B34-2.9)</f>
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:61">
-      <c r="A37" t="s">
+    <row r="38" spans="1:61" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>30</v>
       </c>
-      <c r="B37">
+      <c r="B38">
         <v>8.7999999999999995E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:61">
-      <c r="A38" t="s">
+    <row r="39" spans="1:61" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>31</v>
       </c>
-      <c r="B38">
+      <c r="B39">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:61">
-      <c r="A40" t="s">
+    <row r="41" spans="1:61" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:61">
-      <c r="A41" t="s">
+    <row r="42" spans="1:61" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>33</v>
       </c>
-      <c r="B41">
+      <c r="B42">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:61">
-      <c r="A42" t="s">
+    <row r="43" spans="1:61" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>34</v>
       </c>
-      <c r="B42">
+      <c r="B43">
         <v>2.6700000000000001E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:61">
-      <c r="A43" t="s">
+    <row r="44" spans="1:61" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>35</v>
       </c>
-      <c r="B43">
+      <c r="B44">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:61">
-      <c r="A45" t="s">
+    <row r="46" spans="1:61" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:61">
-      <c r="A46" t="s">
+    <row r="47" spans="1:61" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>37</v>
       </c>
-      <c r="B46">
+      <c r="B47">
         <v>6.7464341725285301E-2</v>
       </c>
-      <c r="C46">
+      <c r="C47">
         <v>6.2569715279821095E-2</v>
       </c>
-      <c r="D46">
+      <c r="D47">
         <v>5.8044680770733E-2</v>
       </c>
-      <c r="E46">
+      <c r="E47">
         <v>5.3860265676456999E-2</v>
       </c>
-      <c r="F46">
+      <c r="F47">
         <v>4.9989849998548802E-2</v>
       </c>
-      <c r="G46">
+      <c r="G47">
         <v>4.6408968795781699E-2</v>
       </c>
-      <c r="H46">
+      <c r="H47">
         <v>4.3095131821452498E-2</v>
       </c>
-      <c r="I46">
+      <c r="I47">
         <v>4.0027658737787797E-2</v>
       </c>
-      <c r="J46">
+      <c r="J47">
         <v>3.7187528521428398E-2</v>
       </c>
-      <c r="K46">
+      <c r="K47">
         <v>3.4557241800832299E-2</v>
       </c>
-      <c r="L46">
+      <c r="L47">
         <v>3.2120694981384701E-2</v>
       </c>
-      <c r="M46">
+      <c r="M47">
         <v>2.9863065118155601E-2</v>
       </c>
-      <c r="N46">
+      <c r="N47">
         <v>2.7770704590669899E-2</v>
       </c>
-      <c r="O46">
+      <c r="O47">
         <v>2.5831044719661599E-2</v>
       </c>
-      <c r="P46">
+      <c r="P47">
         <v>2.4032507543431399E-2</v>
       </c>
-      <c r="Q46">
+      <c r="Q47">
         <v>2.2364425041868901E-2</v>
       </c>
-      <c r="R46">
+      <c r="R47">
         <v>2.0816965160129201E-2</v>
       </c>
-      <c r="S46">
+      <c r="S47">
         <v>1.93810640419734E-2</v>
       </c>
-      <c r="T46">
+      <c r="T47">
         <v>1.80483639354765E-2</v>
       </c>
-      <c r="U46">
+      <c r="U47">
         <v>1.68111562816485E-2</v>
       </c>
-      <c r="V46">
+      <c r="V47">
         <v>1.5662329539992401E-2</v>
       </c>
-      <c r="W46">
+      <c r="W47">
         <v>1.45953213445188E-2</v>
       </c>
-      <c r="X46">
+      <c r="X47">
         <v>1.36040746196468E-2</v>
       </c>
-      <c r="Y46">
+      <c r="Y47">
         <v>1.26829973180606E-2</v>
       </c>
-      <c r="Z46">
+      <c r="Z47">
         <v>1.1826925472286601E-2</v>
       </c>
-      <c r="AA46">
+      <c r="AA47">
         <v>1.10310892787563E-2</v>
       </c>
-      <c r="AB46">
+      <c r="AB47">
         <v>1.0291081957698499E-2</v>
       </c>
-      <c r="AC46">
+      <c r="AC47">
         <v>9.6028311545694797E-3</v>
       </c>
-      <c r="AD46">
+      <c r="AD47">
         <v>8.9625726690923703E-3</v>
       </c>
-      <c r="AE46">
+      <c r="AE47">
         <v>8.3668263165196499E-3</v>
       </c>
-      <c r="AF46">
+      <c r="AF47">
         <v>7.8123737426217801E-3</v>
       </c>
-      <c r="AG46">
+      <c r="AG47">
         <v>7.2962380292947698E-3</v>
       </c>
-      <c r="AH46">
+      <c r="AH47">
         <v>6.8156649417028502E-3</v>
       </c>
-      <c r="AI46">
+      <c r="AI47">
         <v>6.3681056806564199E-3</v>
       </c>
-      <c r="AJ46">
+      <c r="AJ47">
         <v>5.9512010155824101E-3</v>
       </c>
-      <c r="AK46">
+      <c r="AK47">
         <v>5.5627666840751197E-3</v>
       </c>
-      <c r="AL46">
+      <c r="AL47">
         <v>5.2007799537141597E-3</v>
       </c>
-      <c r="AM46">
+      <c r="AM47">
         <v>4.8633672506862898E-3</v>
       </c>
-      <c r="AN46">
+      <c r="AN47">
         <v>4.5487927678251796E-3</v>
       </c>
-      <c r="AO46">
+      <c r="AO47">
         <v>4.2554479720577501E-3</v>
       </c>
-      <c r="AP46">
+      <c r="AP47">
         <v>3.9818419379800199E-3</v>
       </c>
-      <c r="AQ46">
+      <c r="AQ47">
         <v>3.7265924404363501E-3</v>
       </c>
-      <c r="AR46">
+      <c r="AR47">
         <v>3.4884177445959298E-3</v>
       </c>
-      <c r="AS46">
+      <c r="AS47">
         <v>3.2661290371562299E-3</v>
       </c>
-      <c r="AT46">
+      <c r="AT47">
         <v>3.05862344699737E-3</v>
       </c>
-      <c r="AU46">
+      <c r="AU47">
         <v>2.8648776079039798E-3</v>
       </c>
-      <c r="AV46">
+      <c r="AV47">
         <v>2.6839417198961401E-3</v>
       </c>
-      <c r="AW46">
+      <c r="AW47">
         <v>2.5149340693019499E-3</v>
       </c>
-      <c r="AX46">
+      <c r="AX47">
         <v>2.3570359709896402E-3</v>
       </c>
-      <c r="AY46">
+      <c r="AY47">
         <v>2.2094870991837198E-3</v>
       </c>
-      <c r="AZ46">
+      <c r="AZ47">
         <v>2.07158117604244E-3</v>
       </c>
-      <c r="BA46">
+      <c r="BA47">
         <v>1.94266198969363E-3</v>
       </c>
-      <c r="BB46">
+      <c r="BB47">
         <v>1.82211971573439E-3</v>
       </c>
-      <c r="BC46">
+      <c r="BC47">
         <v>1.7093875183142001E-3</v>
       </c>
-      <c r="BD46">
+      <c r="BD47">
         <v>1.60393840885853E-3</v>
       </c>
-      <c r="BE46">
+      <c r="BE47">
         <v>1.5052823422654501E-3</v>
       </c>
-      <c r="BF46">
+      <c r="BF47">
         <v>1.4129635320353101E-3</v>
       </c>
-      <c r="BG46">
+      <c r="BG47">
         <v>1.3265579672862E-3</v>
       </c>
-      <c r="BH46">
+      <c r="BH47">
         <v>1.24567111597624E-3</v>
       </c>
-      <c r="BI46">
+      <c r="BI47">
         <v>1.1699357999096101E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:61">
-      <c r="A47" t="s">
+    <row r="48" spans="1:61" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>38</v>
       </c>
-      <c r="B47">
+      <c r="B48">
         <v>3.8976322961607419E-2</v>
       </c>
-      <c r="C47">
+      <c r="C48">
         <v>4.1763681789451099E-2</v>
       </c>
-      <c r="D47">
+      <c r="D48">
         <v>4.4750376230533087E-2</v>
       </c>
-      <c r="E47">
+      <c r="E48">
         <v>4.7950661602123634E-2</v>
       </c>
-      <c r="F47">
+      <c r="F48">
         <v>5.1379812681496398E-2</v>
       </c>
-      <c r="G47">
+      <c r="G48">
         <v>5.5054196604270633E-2</v>
       </c>
-      <c r="H47">
+      <c r="H48">
         <v>5.899135098992387E-2</v>
       </c>
-      <c r="I47">
+      <c r="I48">
         <v>6.3210067648711482E-2</v>
       </c>
-      <c r="J47">
+      <c r="J48">
         <v>6.7730482265692796E-2</v>
       </c>
-      <c r="K47">
+      <c r="K48">
         <v>7.2574170518508646E-2</v>
       </c>
-      <c r="L47">
+      <c r="L48">
         <v>7.7764251047267016E-2</v>
       </c>
-      <c r="M47">
+      <c r="M48">
         <v>8.3325495801654187E-2</v>
       </c>
-      <c r="N47">
+      <c r="N48">
         <v>8.9284448280865125E-2</v>
       </c>
-      <c r="O47">
+      <c r="O48">
         <v>9.5669550213232396E-2</v>
       </c>
-      <c r="P47">
+      <c r="P48">
         <v>0.10251127732033963</v>
       </c>
-      <c r="Q47">
+      <c r="Q48">
         <v>0.10984228476523736</v>
       </c>
-      <c r="R47">
+      <c r="R48">
         <v>0.117697563017892</v>
       </c>
-      <c r="S47">
+      <c r="S48">
         <v>0.12611460486164955</v>
       </c>
-      <c r="T47">
+      <c r="T48">
         <v>0.13513358434653355</v>
       </c>
-      <c r="U47">
+      <c r="U48">
         <v>0.14479754853404289</v>
       </c>
-      <c r="V47">
+      <c r="V48">
         <v>0.15515262296177337</v>
       </c>
-      <c r="W47">
+      <c r="W48">
         <v>0.16624823179229323</v>
       </c>
-      <c r="X47">
+      <c r="X48">
         <v>0.1781373337217208</v>
       </c>
-      <c r="Y47">
+      <c r="Y48">
         <v>0.19087667473632991</v>
       </c>
-      <c r="Z47">
+      <c r="Z48">
         <v>0.20452705896799719</v>
       </c>
-      <c r="AA47">
+      <c r="AA48">
         <v>0.21915363890262818</v>
       </c>
-      <c r="AB47">
+      <c r="AB48">
         <v>0.23482622635097872</v>
       </c>
-      <c r="AC47">
+      <c r="AC48">
         <v>0.25161962565837315</v>
       </c>
-      <c r="AD47">
+      <c r="AD48">
         <v>0.26961399073885811</v>
       </c>
-      <c r="AE47">
+      <c r="AE48">
         <v>0.28889520764374826</v>
       </c>
-      <c r="AF47">
+      <c r="AF48">
         <v>0.30955530449675772</v>
       </c>
-      <c r="AG47">
+      <c r="AG48">
         <v>0.33169289073156716</v>
       </c>
-      <c r="AH47">
+      <c r="AH48">
         <v>0.35541362775511665</v>
       </c>
-      <c r="AI47">
+      <c r="AI48">
         <v>0.38083073325887362</v>
       </c>
-      <c r="AJ47">
+      <c r="AJ48">
         <v>0.40806552160225951</v>
       </c>
-      <c r="AK47">
+      <c r="AK48">
         <v>0.43724798283859007</v>
       </c>
-      <c r="AL47">
+      <c r="AL48">
         <v>0.4685174031514211</v>
       </c>
-      <c r="AM47">
+      <c r="AM48">
         <v>0.50202302965577317</v>
       </c>
-      <c r="AN47">
+      <c r="AN48">
         <v>0.53792478274989508</v>
       </c>
-      <c r="AO47">
+      <c r="AO48">
         <v>0.5763940194045446</v>
       </c>
-      <c r="AP47">
+      <c r="AP48">
         <v>0.6176143510369575</v>
       </c>
-      <c r="AQ47">
+      <c r="AQ48">
         <v>0.66178251988334214</v>
       </c>
-      <c r="AR47">
+      <c r="AR48">
         <v>0.70910933803147658</v>
       </c>
-      <c r="AS47">
+      <c r="AS48">
         <v>0.75982069362106486</v>
       </c>
-      <c r="AT47">
+      <c r="AT48">
         <v>0.81415862898843427</v>
       </c>
-      <c r="AU47">
-        <v>1</v>
-      </c>
-      <c r="AV47">
-        <v>1</v>
-      </c>
-      <c r="AW47">
-        <v>1</v>
-      </c>
-      <c r="AX47">
-        <v>1</v>
-      </c>
-      <c r="AY47">
-        <v>1</v>
-      </c>
-      <c r="AZ47">
-        <v>1</v>
-      </c>
-      <c r="BA47">
-        <v>1</v>
-      </c>
-      <c r="BB47">
-        <v>1</v>
-      </c>
-      <c r="BC47">
-        <v>1</v>
-      </c>
-      <c r="BD47">
-        <v>1</v>
-      </c>
-      <c r="BE47">
-        <v>1</v>
-      </c>
-      <c r="BF47">
-        <v>1</v>
-      </c>
-      <c r="BG47">
-        <v>1</v>
-      </c>
-      <c r="BH47">
-        <v>1</v>
-      </c>
-      <c r="BI47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:61">
-      <c r="A48" t="s">
+      <c r="AU48">
+        <v>1</v>
+      </c>
+      <c r="AV48">
+        <v>1</v>
+      </c>
+      <c r="AW48">
+        <v>1</v>
+      </c>
+      <c r="AX48">
+        <v>1</v>
+      </c>
+      <c r="AY48">
+        <v>1</v>
+      </c>
+      <c r="AZ48">
+        <v>1</v>
+      </c>
+      <c r="BA48">
+        <v>1</v>
+      </c>
+      <c r="BB48">
+        <v>1</v>
+      </c>
+      <c r="BC48">
+        <v>1</v>
+      </c>
+      <c r="BD48">
+        <v>1</v>
+      </c>
+      <c r="BE48">
+        <v>1</v>
+      </c>
+      <c r="BF48">
+        <v>1</v>
+      </c>
+      <c r="BG48">
+        <v>1</v>
+      </c>
+      <c r="BH48">
+        <v>1</v>
+      </c>
+      <c r="BI48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>39</v>
       </c>
-      <c r="B48">
+      <c r="B49">
         <v>2.8</v>
       </c>
     </row>
-    <row r="49" spans="1:68">
-      <c r="A49" t="s">
+    <row r="50" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>40</v>
       </c>
-      <c r="B49">
-        <v>1</v>
-      </c>
-      <c r="C49">
-        <v>1</v>
-      </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-      <c r="E49">
-        <v>1</v>
-      </c>
-      <c r="F49">
-        <v>1</v>
-      </c>
-      <c r="G49">
-        <v>1</v>
-      </c>
-      <c r="H49">
-        <v>1</v>
-      </c>
-      <c r="I49">
-        <v>1</v>
-      </c>
-      <c r="J49">
-        <v>1</v>
-      </c>
-      <c r="K49">
-        <v>1</v>
-      </c>
-      <c r="L49">
-        <v>1</v>
-      </c>
-      <c r="M49">
-        <v>1</v>
-      </c>
-      <c r="N49">
-        <v>1</v>
-      </c>
-      <c r="O49">
-        <v>1</v>
-      </c>
-      <c r="P49">
-        <v>1</v>
-      </c>
-      <c r="Q49">
-        <v>1</v>
-      </c>
-      <c r="R49">
-        <v>1</v>
-      </c>
-      <c r="S49">
-        <v>1</v>
-      </c>
-      <c r="T49">
-        <v>1</v>
-      </c>
-      <c r="U49">
-        <v>1</v>
-      </c>
-      <c r="V49">
-        <v>1</v>
-      </c>
-      <c r="W49">
-        <v>1</v>
-      </c>
-      <c r="X49">
-        <v>1</v>
-      </c>
-      <c r="Y49">
-        <v>1</v>
-      </c>
-      <c r="Z49">
-        <v>1</v>
-      </c>
-      <c r="AA49">
-        <v>1</v>
-      </c>
-      <c r="AB49">
-        <v>1</v>
-      </c>
-      <c r="AC49">
-        <v>1</v>
-      </c>
-      <c r="AD49">
-        <v>1</v>
-      </c>
-      <c r="AE49">
-        <v>1</v>
-      </c>
-      <c r="AF49">
-        <v>1</v>
-      </c>
-      <c r="AG49">
-        <v>1</v>
-      </c>
-      <c r="AH49">
-        <v>1</v>
-      </c>
-      <c r="AI49">
-        <v>1</v>
-      </c>
-      <c r="AJ49">
-        <v>1</v>
-      </c>
-      <c r="AK49">
-        <v>1</v>
-      </c>
-      <c r="AL49">
-        <v>1</v>
-      </c>
-      <c r="AM49">
-        <v>1</v>
-      </c>
-      <c r="AN49">
-        <v>1</v>
-      </c>
-      <c r="AO49">
-        <v>1</v>
-      </c>
-      <c r="AP49">
-        <v>1</v>
-      </c>
-      <c r="AQ49">
-        <v>1</v>
-      </c>
-      <c r="AR49">
-        <v>1</v>
-      </c>
-      <c r="AS49">
-        <v>1</v>
-      </c>
-      <c r="AT49">
-        <v>1</v>
-      </c>
-      <c r="AU49">
-        <v>1</v>
-      </c>
-      <c r="AV49">
-        <v>1</v>
-      </c>
-      <c r="AW49">
-        <v>1</v>
-      </c>
-      <c r="AX49">
-        <v>1</v>
-      </c>
-      <c r="AY49">
-        <v>1</v>
-      </c>
-      <c r="AZ49">
-        <v>1</v>
-      </c>
-      <c r="BA49">
-        <v>1</v>
-      </c>
-      <c r="BB49">
-        <v>1</v>
-      </c>
-      <c r="BC49">
-        <v>1</v>
-      </c>
-      <c r="BD49">
-        <v>1</v>
-      </c>
-      <c r="BE49">
-        <v>1</v>
-      </c>
-      <c r="BF49">
-        <v>1</v>
-      </c>
-      <c r="BG49">
-        <v>1</v>
-      </c>
-      <c r="BH49">
-        <v>1</v>
-      </c>
-      <c r="BI49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:68">
-      <c r="A50" t="s">
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="H50">
+        <v>1</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+      <c r="K50">
+        <v>1</v>
+      </c>
+      <c r="L50">
+        <v>1</v>
+      </c>
+      <c r="M50">
+        <v>1</v>
+      </c>
+      <c r="N50">
+        <v>1</v>
+      </c>
+      <c r="O50">
+        <v>1</v>
+      </c>
+      <c r="P50">
+        <v>1</v>
+      </c>
+      <c r="Q50">
+        <v>1</v>
+      </c>
+      <c r="R50">
+        <v>1</v>
+      </c>
+      <c r="S50">
+        <v>1</v>
+      </c>
+      <c r="T50">
+        <v>1</v>
+      </c>
+      <c r="U50">
+        <v>1</v>
+      </c>
+      <c r="V50">
+        <v>1</v>
+      </c>
+      <c r="W50">
+        <v>1</v>
+      </c>
+      <c r="X50">
+        <v>1</v>
+      </c>
+      <c r="Y50">
+        <v>1</v>
+      </c>
+      <c r="Z50">
+        <v>1</v>
+      </c>
+      <c r="AA50">
+        <v>1</v>
+      </c>
+      <c r="AB50">
+        <v>1</v>
+      </c>
+      <c r="AC50">
+        <v>1</v>
+      </c>
+      <c r="AD50">
+        <v>1</v>
+      </c>
+      <c r="AE50">
+        <v>1</v>
+      </c>
+      <c r="AF50">
+        <v>1</v>
+      </c>
+      <c r="AG50">
+        <v>1</v>
+      </c>
+      <c r="AH50">
+        <v>1</v>
+      </c>
+      <c r="AI50">
+        <v>1</v>
+      </c>
+      <c r="AJ50">
+        <v>1</v>
+      </c>
+      <c r="AK50">
+        <v>1</v>
+      </c>
+      <c r="AL50">
+        <v>1</v>
+      </c>
+      <c r="AM50">
+        <v>1</v>
+      </c>
+      <c r="AN50">
+        <v>1</v>
+      </c>
+      <c r="AO50">
+        <v>1</v>
+      </c>
+      <c r="AP50">
+        <v>1</v>
+      </c>
+      <c r="AQ50">
+        <v>1</v>
+      </c>
+      <c r="AR50">
+        <v>1</v>
+      </c>
+      <c r="AS50">
+        <v>1</v>
+      </c>
+      <c r="AT50">
+        <v>1</v>
+      </c>
+      <c r="AU50">
+        <v>1</v>
+      </c>
+      <c r="AV50">
+        <v>1</v>
+      </c>
+      <c r="AW50">
+        <v>1</v>
+      </c>
+      <c r="AX50">
+        <v>1</v>
+      </c>
+      <c r="AY50">
+        <v>1</v>
+      </c>
+      <c r="AZ50">
+        <v>1</v>
+      </c>
+      <c r="BA50">
+        <v>1</v>
+      </c>
+      <c r="BB50">
+        <v>1</v>
+      </c>
+      <c r="BC50">
+        <v>1</v>
+      </c>
+      <c r="BD50">
+        <v>1</v>
+      </c>
+      <c r="BE50">
+        <v>1</v>
+      </c>
+      <c r="BF50">
+        <v>1</v>
+      </c>
+      <c r="BG50">
+        <v>1</v>
+      </c>
+      <c r="BH50">
+        <v>1</v>
+      </c>
+      <c r="BI50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>41</v>
       </c>
-      <c r="B50">
+      <c r="B51">
         <v>344</v>
       </c>
-      <c r="C50">
+      <c r="C51">
         <v>335.4</v>
       </c>
-      <c r="D50">
+      <c r="D51">
         <v>327.01499999999999</v>
       </c>
-      <c r="E50">
+      <c r="E51">
         <v>318.83962499999899</v>
       </c>
-      <c r="F50">
+      <c r="F51">
         <v>310.86863437499898</v>
       </c>
-      <c r="G50">
+      <c r="G51">
         <v>303.096918515624</v>
       </c>
-      <c r="H50">
+      <c r="H51">
         <v>295.51949555273399</v>
       </c>
-      <c r="I50">
+      <c r="I51">
         <v>288.13150816391601</v>
       </c>
-      <c r="J50">
+      <c r="J51">
         <v>280.92822045981802</v>
       </c>
-      <c r="K50">
+      <c r="K51">
         <v>273.90501494832199</v>
       </c>
-      <c r="L50">
+      <c r="L51">
         <v>267.05738957461398</v>
       </c>
-      <c r="M50">
+      <c r="M51">
         <v>260.38095483524899</v>
       </c>
-      <c r="N50">
+      <c r="N51">
         <v>253.87143096436699</v>
       </c>
-      <c r="O50">
+      <c r="O51">
         <v>247.52464519025801</v>
       </c>
-      <c r="P50">
+      <c r="P51">
         <v>241.33652906050199</v>
       </c>
-      <c r="Q50">
+      <c r="Q51">
         <v>235.30311583398901</v>
       </c>
-      <c r="R50">
+      <c r="R51">
         <v>229.42053793813901</v>
       </c>
-      <c r="S50">
+      <c r="S51">
         <v>223.68502448968599</v>
       </c>
-      <c r="T50">
+      <c r="T51">
         <v>218.09289887744399</v>
       </c>
-      <c r="U50">
+      <c r="U51">
         <v>212.640576405508</v>
       </c>
-      <c r="V50">
+      <c r="V51">
         <v>207.32456199537</v>
       </c>
-      <c r="W50">
+      <c r="W51">
         <v>202.14144794548599</v>
       </c>
-      <c r="X50">
+      <c r="X51">
         <v>197.08791174684899</v>
       </c>
-      <c r="Y50">
+      <c r="Y51">
         <v>192.16071395317701</v>
       </c>
-      <c r="Z50">
+      <c r="Z51">
         <v>187.356696104348</v>
       </c>
-      <c r="AA50">
+      <c r="AA51">
         <v>182.67277870173899</v>
       </c>
-      <c r="AB50">
+      <c r="AB51">
         <v>178.10595923419601</v>
       </c>
-      <c r="AC50">
+      <c r="AC51">
         <v>173.653310253341</v>
       </c>
-      <c r="AD50">
+      <c r="AD51">
         <v>169.31197749700701</v>
       </c>
-      <c r="AE50">
+      <c r="AE51">
         <v>165.07917805958201</v>
       </c>
-      <c r="AF50">
+      <c r="AF51">
         <v>160.952198608092</v>
       </c>
-      <c r="AG50">
+      <c r="AG51">
         <v>156.92839364289</v>
       </c>
-      <c r="AH50">
+      <c r="AH51">
         <v>153.00518380181799</v>
       </c>
-      <c r="AI50">
+      <c r="AI51">
         <v>149.18005420677201</v>
       </c>
-      <c r="AJ50">
+      <c r="AJ51">
         <v>145.45055285160299</v>
       </c>
-      <c r="AK50">
+      <c r="AK51">
         <v>141.81428903031301</v>
       </c>
-      <c r="AL50">
+      <c r="AL51">
         <v>138.268931804555</v>
       </c>
-      <c r="AM50">
+      <c r="AM51">
         <v>134.81220850944101</v>
       </c>
-      <c r="AN50">
+      <c r="AN51">
         <v>131.44190329670499</v>
       </c>
-      <c r="AO50">
+      <c r="AO51">
         <v>128.15585571428801</v>
       </c>
-      <c r="AP50">
+      <c r="AP51">
         <v>124.95195932143</v>
       </c>
-      <c r="AQ50">
+      <c r="AQ51">
         <v>121.82816033839499</v>
       </c>
-      <c r="AR50">
+      <c r="AR51">
         <v>118.782456329935</v>
       </c>
-      <c r="AS50">
+      <c r="AS51">
         <v>115.812894921686</v>
       </c>
-      <c r="AT50">
+      <c r="AT51">
         <v>112.917572548644</v>
       </c>
-      <c r="AU50">
+      <c r="AU51">
         <v>110.094633234928</v>
       </c>
-      <c r="AV50">
+      <c r="AV51">
         <v>107.34226740405499</v>
       </c>
-      <c r="AW50">
+      <c r="AW51">
         <v>104.658710718953</v>
       </c>
-      <c r="AX50">
+      <c r="AX51">
         <v>102.04224295098</v>
       </c>
-      <c r="AY50">
+      <c r="AY51">
         <v>99.491186877205493</v>
       </c>
-      <c r="AZ50">
+      <c r="AZ51">
         <v>97.003907205275397</v>
       </c>
-      <c r="BA50">
+      <c r="BA51">
         <v>94.578809525143498</v>
       </c>
-      <c r="BB50">
+      <c r="BB51">
         <v>92.214339287014894</v>
       </c>
-      <c r="BC50">
+      <c r="BC51">
         <v>89.908980804839501</v>
       </c>
-      <c r="BD50">
+      <c r="BD51">
         <v>87.661256284718505</v>
       </c>
-      <c r="BE50">
+      <c r="BE51">
         <v>85.469724877600598</v>
       </c>
-      <c r="BF50">
+      <c r="BF51">
         <v>83.332981755660498</v>
       </c>
-      <c r="BG50">
+      <c r="BG51">
         <v>81.249657211769005</v>
       </c>
-      <c r="BH50">
+      <c r="BH51">
         <v>79.218415781474803</v>
       </c>
-      <c r="BI50">
+      <c r="BI51">
         <v>77.237955386937898</v>
       </c>
     </row>
-    <row r="51" spans="1:68" s="2" customFormat="1">
-      <c r="A51" s="2" t="s">
+    <row r="52" spans="1:68" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B52" s="3">
         <v>0.25795812594001399</v>
       </c>
-      <c r="C51" s="4">
+      <c r="C52" s="4">
         <v>0.25511678812409011</v>
       </c>
-      <c r="D51" s="4">
+      <c r="D52" s="4">
         <v>0.25252802427428017</v>
       </c>
-      <c r="E51" s="4">
+      <c r="E52" s="4">
         <v>0.25020956772436381</v>
       </c>
-      <c r="F51" s="4">
+      <c r="F52" s="4">
         <v>0.2481552469823238</v>
       </c>
-      <c r="G51" s="4">
+      <c r="G52" s="4">
         <v>0.24634814996173846</v>
       </c>
-      <c r="H51" s="4">
+      <c r="H52" s="4">
         <v>0.24476698996275215</v>
       </c>
-      <c r="I51" s="4">
+      <c r="I52" s="4">
         <v>0.24338909993327604</v>
       </c>
-      <c r="J51" s="4">
+      <c r="J52" s="4">
         <v>0.24219227400546323</v>
       </c>
-      <c r="K51" s="4">
+      <c r="K52" s="4">
         <v>0.24115588214534792</v>
       </c>
-      <c r="L51" s="4">
+      <c r="L52" s="4">
         <v>0.24026150867249696</v>
       </c>
-      <c r="M51" s="4">
+      <c r="M52" s="4">
         <v>0.23949311141371168</v>
       </c>
-      <c r="N51" s="4">
+      <c r="N52" s="4">
         <v>0.23883689427227053</v>
       </c>
-      <c r="O51" s="4">
+      <c r="O52" s="4">
         <v>0.23828078897803687</v>
       </c>
-      <c r="P51" s="4">
+      <c r="P52" s="4">
         <v>0.23781401494219165</v>
       </c>
-      <c r="Q51" s="4">
+      <c r="Q52" s="4">
         <v>0.23742642550701054</v>
       </c>
-      <c r="R51" s="4">
+      <c r="R52" s="4">
         <v>0.23710785652392138</v>
       </c>
-      <c r="S51" s="4">
+      <c r="S52" s="4">
         <v>0.23684703205480417</v>
       </c>
-      <c r="T51" s="4">
+      <c r="T52" s="4">
         <v>0.23662980779339443</v>
       </c>
-      <c r="U51" s="4">
+      <c r="U52" s="4">
         <v>0.2364766752320539</v>
       </c>
-      <c r="V51" s="4">
+      <c r="V52" s="4">
         <v>0.23638152967662066</v>
       </c>
-      <c r="W51" s="4">
+      <c r="W52" s="4">
         <v>0.23634043118378459</v>
       </c>
-      <c r="X51" s="4">
+      <c r="X52" s="4">
         <v>0.23635103874149985</v>
       </c>
-      <c r="Y51" s="4">
+      <c r="Y52" s="4">
         <v>0.23641234945292194</v>
       </c>
-      <c r="Z51" s="4">
+      <c r="Z52" s="4">
         <v>0.23652439593263558</v>
       </c>
-      <c r="AA51" s="4">
+      <c r="AA52" s="4">
         <v>0.23668823907344283</v>
       </c>
-      <c r="AB51" s="4">
+      <c r="AB52" s="4">
         <v>0.23690591864236035</v>
       </c>
-      <c r="AC51" s="4">
+      <c r="AC52" s="4">
         <v>0.23718064345108103</v>
       </c>
-      <c r="AD51" s="4">
+      <c r="AD52" s="4">
         <v>0.23751707143668549</v>
       </c>
-      <c r="AE51" s="4">
+      <c r="AE52" s="4">
         <v>0.23748240011358901</v>
       </c>
-      <c r="AF51" s="4">
+      <c r="AF52" s="4">
         <v>0.23778955120526299</v>
       </c>
-      <c r="AG51" s="4">
+      <c r="AG52" s="4">
         <v>0.23813080763560601</v>
       </c>
-      <c r="AH51" s="4">
+      <c r="AH52" s="4">
         <v>0.238505650017792</v>
       </c>
-      <c r="AI51" s="4">
+      <c r="AI52" s="4">
         <v>0.238913716179254</v>
       </c>
-      <c r="AJ51" s="4">
+      <c r="AJ52" s="4">
         <v>0.23935495851553501</v>
       </c>
-      <c r="AK51" s="4">
+      <c r="AK52" s="4">
         <v>0.239829922012531</v>
       </c>
-      <c r="AL51" s="4">
+      <c r="AL52" s="4">
         <v>0.24034033132468099</v>
       </c>
-      <c r="AM51" s="4">
+      <c r="AM52" s="4">
         <v>0.24089009911753201</v>
       </c>
-      <c r="AN51" s="4">
+      <c r="AN52" s="4">
         <v>0.24148736410706301</v>
       </c>
-      <c r="AO51" s="4">
+      <c r="AO52" s="4">
         <v>0.24214788078489</v>
       </c>
-      <c r="AP51" s="4">
+      <c r="AP52" s="4">
         <v>0.24290140488952799</v>
       </c>
-      <c r="AQ51" s="4">
+      <c r="AQ52" s="4">
         <v>0.24380273491736701</v>
       </c>
-      <c r="AR51" s="4">
+      <c r="AR52" s="4">
         <v>0.24495135804013099</v>
       </c>
-      <c r="AS51" s="4">
+      <c r="AS52" s="4">
         <v>0.24652554216615</v>
       </c>
-      <c r="AT51" s="4">
+      <c r="AT52" s="4">
         <v>0.24884063584274799</v>
       </c>
-      <c r="AU51" s="4">
+      <c r="AU52" s="4">
         <v>0.24710573688184301</v>
       </c>
-      <c r="AV51" s="4">
+      <c r="AV52" s="4">
         <v>0.24651311712087301</v>
       </c>
-      <c r="AW51" s="4">
+      <c r="AW52" s="4">
         <v>0.24573792403446401</v>
       </c>
-      <c r="AX51" s="4">
+      <c r="AX52" s="4">
         <v>0.244467711019796</v>
       </c>
-      <c r="AY51" s="4">
+      <c r="AY52" s="4">
         <v>0.242206858344204</v>
       </c>
-      <c r="AZ51" s="4">
+      <c r="AZ52" s="4">
         <v>0.258278145695364</v>
       </c>
-      <c r="BA51" s="4">
+      <c r="BA52" s="4">
         <v>0.258278145695364</v>
       </c>
-      <c r="BB51" s="4">
+      <c r="BB52" s="4">
         <v>0.258278145695364</v>
       </c>
-      <c r="BC51" s="4">
+      <c r="BC52" s="4">
         <v>0.258278145695364</v>
       </c>
-      <c r="BD51" s="4">
+      <c r="BD52" s="4">
         <v>0.258278145695364</v>
       </c>
-      <c r="BE51" s="4">
+      <c r="BE52" s="4">
         <v>0.258278145695364</v>
       </c>
-      <c r="BF51" s="4">
+      <c r="BF52" s="4">
         <v>0.258278145695364</v>
       </c>
-      <c r="BG51" s="4">
+      <c r="BG52" s="4">
         <v>0.258278145695364</v>
       </c>
-      <c r="BH51" s="4">
+      <c r="BH52" s="4">
         <v>0.258278145695364</v>
       </c>
-      <c r="BI51" s="4">
+      <c r="BI52" s="4">
         <v>0.258278145695364</v>
       </c>
-      <c r="BJ51" s="5"/>
-      <c r="BK51" s="5"/>
-      <c r="BL51" s="5"/>
-      <c r="BM51" s="5"/>
-      <c r="BN51" s="5"/>
-      <c r="BO51" s="5"/>
-      <c r="BP51" s="5"/>
-    </row>
-    <row r="53" spans="1:68">
-      <c r="A53" t="s">
+      <c r="BJ52" s="5"/>
+      <c r="BK52" s="5"/>
+      <c r="BL52" s="5"/>
+      <c r="BM52" s="5"/>
+      <c r="BN52" s="5"/>
+      <c r="BO52" s="5"/>
+      <c r="BP52" s="5"/>
+    </row>
+    <row r="54" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="1:68">
-      <c r="A54" t="s">
+    <row r="55" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
         <v>44</v>
       </c>
-      <c r="B54">
+      <c r="B55">
         <v>1.45</v>
       </c>
     </row>
-    <row r="55" spans="1:68">
-      <c r="A55" t="s">
+    <row r="56" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>45</v>
       </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
-      <c r="C55">
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
         <v>0.92826032540563896</v>
       </c>
-      <c r="D55">
+      <c r="D56">
         <v>0.86166723172218396</v>
       </c>
-      <c r="E55">
+      <c r="E56">
         <v>0.79985150490981105</v>
       </c>
-      <c r="F55">
+      <c r="F56">
         <v>0.74247041822377202</v>
       </c>
-      <c r="G55">
+      <c r="G56">
         <v>0.68920583202445995</v>
       </c>
-      <c r="H55">
+      <c r="H56">
         <v>0.63976242990649002</v>
       </c>
-      <c r="I55">
+      <c r="I56">
         <v>0.59386608136730101</v>
       </c>
-      <c r="J55">
+      <c r="J56">
         <v>0.551262321937383</v>
       </c>
-      <c r="K55">
+      <c r="K56">
         <v>0.511714942345464</v>
       </c>
-      <c r="L55">
+      <c r="L56">
         <v>0.47500467889652798</v>
       </c>
-      <c r="M55">
+      <c r="M56">
         <v>0.44092799780169301</v>
       </c>
-      <c r="N55">
+      <c r="N56">
         <v>0.40929596671985702</v>
       </c>
-      <c r="O55">
+      <c r="O56">
         <v>0.37993320725459001</v>
       </c>
-      <c r="P55">
+      <c r="P56">
         <v>0.35267692259855399</v>
       </c>
-      <c r="Q55">
+      <c r="Q56">
         <v>0.32737599493439301</v>
       </c>
-      <c r="R55">
+      <c r="R56">
         <v>0.30389014758779498</v>
       </c>
-      <c r="S55">
+      <c r="S56">
         <v>0.28208916728741501</v>
       </c>
-      <c r="T55">
+      <c r="T56">
         <v>0.26185218221962098</v>
       </c>
-      <c r="U55">
+      <c r="U56">
         <v>0.24306699187536299</v>
       </c>
-      <c r="V55">
+      <c r="V56">
         <v>0.225629444973594</v>
       </c>
-      <c r="W55">
+      <c r="W56">
         <v>0.20944286201228199</v>
       </c>
-      <c r="X55">
+      <c r="X56">
         <v>0.19441749924540999</v>
       </c>
-      <c r="Y55">
+      <c r="Y56">
         <v>0.180470051114095</v>
       </c>
-      <c r="Z55">
+      <c r="Z56">
         <v>0.16752318837314201</v>
       </c>
-      <c r="AA55">
+      <c r="AA56">
         <v>0.155505129352243</v>
       </c>
-      <c r="AB55">
+      <c r="AB56">
         <v>0.14434924197475901</v>
       </c>
-      <c r="AC55">
+      <c r="AC56">
         <v>0.133993674327547</v>
       </c>
-      <c r="AD55">
+      <c r="AD56">
         <v>0.124381011733586</v>
       </c>
-      <c r="AE55">
+      <c r="AE56">
         <v>0.115457958426102</v>
       </c>
-      <c r="AF55">
+      <c r="AF56">
         <v>0.10717504205928401</v>
       </c>
-      <c r="AG55">
+      <c r="AG56">
         <v>9.9486339417314301E-2</v>
       </c>
-      <c r="AH55">
+      <c r="AH56">
         <v>9.2349221800932094E-2</v>
       </c>
-      <c r="AI55">
+      <c r="AI56">
         <v>8.5724118679890896E-2</v>
       </c>
-      <c r="AJ55">
+      <c r="AJ56">
         <v>7.9574298300907204E-2</v>
       </c>
-      <c r="AK55">
+      <c r="AK56">
         <v>7.3865664034725498E-2</v>
       </c>
-      <c r="AL55">
+      <c r="AL56">
         <v>6.8566565333177995E-2</v>
       </c>
-      <c r="AM55">
+      <c r="AM56">
         <v>6.3647622248122898E-2</v>
       </c>
-      <c r="AN55">
+      <c r="AN56">
         <v>5.9081562539337801E-2</v>
       </c>
-      <c r="AO55">
+      <c r="AO56">
         <v>5.4843070468239302E-2</v>
       </c>
-      <c r="AP55">
+      <c r="AP56">
         <v>5.0908646439092299E-2</v>
       </c>
-      <c r="AQ55">
+      <c r="AQ56">
         <v>4.7256476709512503E-2</v>
       </c>
-      <c r="AR55">
+      <c r="AR56">
         <v>4.38663124478961E-2</v>
       </c>
-      <c r="AS55">
+      <c r="AS56">
         <v>4.0719357467229503E-2</v>
       </c>
-      <c r="AT55">
+      <c r="AT56">
         <v>3.7798164012839003E-2</v>
       </c>
-      <c r="AU55">
+      <c r="AU56">
         <v>3.5086536026293698E-2</v>
       </c>
-      <c r="AV55">
+      <c r="AV56">
         <v>3.2569439349124103E-2</v>
       </c>
-      <c r="AW55">
+      <c r="AW56">
         <v>3.0232918368497098E-2</v>
       </c>
-      <c r="AX55">
+      <c r="AX56">
         <v>2.80640186427033E-2</v>
       </c>
-      <c r="AY55">
+      <c r="AY56">
         <v>2.6050715077465699E-2</v>
       </c>
-      <c r="AZ55">
+      <c r="AZ56">
         <v>2.4181845254857899E-2</v>
       </c>
-      <c r="BA55">
+      <c r="BA56">
         <v>2.2447047545183198E-2</v>
       </c>
-      <c r="BB55">
+      <c r="BB56">
         <v>2.08367036586877E-2</v>
       </c>
-      <c r="BC55">
+      <c r="BC56">
         <v>1.93418853185943E-2</v>
       </c>
-      <c r="BD55">
+      <c r="BD56">
         <v>1.79543047597969E-2</v>
       </c>
-      <c r="BE55">
+      <c r="BE56">
         <v>1.6666268778761099E-2</v>
       </c>
-      <c r="BF55">
+      <c r="BF56">
         <v>1.5470636079870599E-2</v>
       </c>
-      <c r="BG55">
+      <c r="BG56">
         <v>1.4360777681732899E-2</v>
       </c>
-      <c r="BH55">
+      <c r="BH56">
         <v>1.33305401639235E-2</v>
       </c>
-      <c r="BI55">
+      <c r="BI56">
         <v>1.23742115503965E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:68">
-      <c r="A56" t="s">
+    <row r="57" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
         <v>47</v>
       </c>
-      <c r="B56">
+      <c r="B57">
         <v>1.6408662000000001E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:68">
-      <c r="A57" t="s">
+    <row r="58" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>48</v>
       </c>
-      <c r="B57">
+      <c r="B58">
         <v>-3855.1068949999999</v>
       </c>
     </row>

</xml_diff>